<commit_message>
fix: longest streak issue recorded
</commit_message>
<xml_diff>
--- a/docs/testing/tests.xlsx
+++ b/docs/testing/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/T7/Dropbox/_Milestone project 2 project/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765DF0AF-C7AB-AE45-ACBD-C23279101C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81709E5-B992-714C-A4A1-ED5BC751E7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="4900" windowWidth="28800" windowHeight="15440" xr2:uid="{D3B9687F-2C93-41C3-BC0D-C0399298551E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="109">
   <si>
     <t>#ID</t>
   </si>
@@ -353,6 +353,18 @@
   </si>
   <si>
     <t>Removed type declaration</t>
+  </si>
+  <si>
+    <t>game_landing.html</t>
+  </si>
+  <si>
+    <t>lomgest streak not persisting until game end screen</t>
+  </si>
+  <si>
+    <t>Edited scripts.js</t>
+  </si>
+  <si>
+    <t>Added function to track streak and update longest streak as to persist until game end screen.</t>
   </si>
 </sst>
 </file>
@@ -418,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -454,6 +466,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1172,9 +1187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E4AF7C-64D1-4828-9043-9C11E87A7910}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1954,15 +1967,28 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">

</xml_diff>